<commit_message>
complete DDT code, update data
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanph\OneDrive\Máy tính\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanph\OneDrive\Máy tính\messy stub\netbean 19\selenium-2-go\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788A5CFE-FEDF-445C-81FC-AF5DCE9F503F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A272FEE2-5F6C-4BFB-94BC-E3A6DDA7AF06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5676" yWindow="5184" windowWidth="14004" windowHeight="9936" xr2:uid="{CEB6D775-E36A-4DF8-BBA1-7606A2A85DC6}"/>
+    <workbookView xWindow="5676" yWindow="2304" windowWidth="14004" windowHeight="9936" xr2:uid="{CEB6D775-E36A-4DF8-BBA1-7606A2A85DC6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>mngr533997</t>
   </si>
@@ -43,13 +43,22 @@
   </si>
   <si>
     <t>AdapYsy</t>
+  </si>
+  <si>
+    <t>usernames</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +86,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -98,7 +115,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -108,6 +125,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,20 +443,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D75301D3-D25A-431E-A53D-0A4355CCFEFE}">
-  <dimension ref="B2:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
     <col min="3" max="3" width="11.88671875" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
+    <row r="1" spans="1:3">
+      <c r="A1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,7 +479,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="26.4">
+    <row r="3" spans="1:3" ht="14.4" customHeight="1">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -451,13 +490,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="1:3">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>